<commit_message>
working on 4x4 field
</commit_message>
<xml_diff>
--- a/Project18/Лист Microsoft Excel.xlsx
+++ b/Project18/Лист Microsoft Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Админ\Desktop\CPP\Project18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F843AB-06FF-4574-B7A0-EBC68F4BFE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00F4B4B-B094-4EBA-B9C8-1F31CD2C8390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11988" yWindow="2484" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11736" yWindow="3348" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="19">
   <si>
     <t>x</t>
   </si>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AB38" sqref="AB38"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,9 +700,9 @@
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8">
         <v>0</v>
       </c>
       <c r="E2" s="9"/>
@@ -712,35 +712,35 @@
       </c>
       <c r="G2" s="7" t="str">
         <f>C2</f>
-        <v>o</v>
-      </c>
-      <c r="H2" s="8" t="str">
+        <v>x</v>
+      </c>
+      <c r="H2" s="8">
         <f>D2</f>
-        <v>x</v>
+        <v>0</v>
       </c>
       <c r="I2" s="7" t="str">
         <f>B3</f>
-        <v>o</v>
-      </c>
-      <c r="J2" s="10" t="str">
+        <v>x</v>
+      </c>
+      <c r="J2" s="10">
         <f>C3</f>
-        <v>x</v>
+        <v>0</v>
       </c>
       <c r="K2" s="7" t="str">
         <f>D3</f>
-        <v>o</v>
-      </c>
-      <c r="L2" s="8" t="str">
+        <v>x</v>
+      </c>
+      <c r="L2" s="8">
         <f>B4</f>
-        <v>x</v>
+        <v>0</v>
       </c>
       <c r="M2" s="7" t="str">
         <f>C4</f>
-        <v>o</v>
-      </c>
-      <c r="N2" s="6" t="str">
+        <v>x</v>
+      </c>
+      <c r="N2" s="6">
         <f>D4</f>
-        <v>x</v>
+        <v>0</v>
       </c>
       <c r="AB2" t="s">
         <v>5</v>
@@ -751,13 +751,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10">
         <v>0</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
@@ -777,13 +777,13 @@
       <c r="A4" s="5">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="8">
         <v>0</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
         <v>0</v>
       </c>
       <c r="E4" s="11"/>

</xml_diff>